<commit_message>
JBTraffic ver 1.2 (GUI)
</commit_message>
<xml_diff>
--- a/Data/BusData.xlsx
+++ b/Data/BusData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoom\OneDrive\문서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssoom\PycharmProjects\JBTraffic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C05E73E6-1AA4-4E21-98F0-1A1D3CBD6D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542112E2-55BA-4055-AA7D-CC8485834BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{C32152F4-31FA-47CC-9FD7-0F0EC0129831}"/>
+    <workbookView xWindow="11055" yWindow="2280" windowWidth="13395" windowHeight="10620" xr2:uid="{C32152F4-31FA-47CC-9FD7-0F0EC0129831}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,12 +453,12 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -480,7 +480,7 @@
         <v>0.34722222222222221</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0.3576388888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -502,7 +502,7 @@
         <v>0.3611111111111111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -513,7 +513,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -524,7 +524,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -535,7 +535,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -546,7 +546,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -557,7 +557,7 @@
         <v>0.47222222222222221</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -568,7 +568,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -579,7 +579,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -590,7 +590,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0.51388888888888884</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -612,7 +612,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -634,7 +634,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -656,7 +656,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -667,7 +667,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -678,7 +678,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -689,7 +689,7 @@
         <v>0.76388888888888884</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -700,7 +700,7 @@
         <v>0.80555555555555558</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -711,7 +711,7 @@
         <v>0.34722222222222221</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -722,7 +722,7 @@
         <v>0.35069444444444442</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -733,7 +733,7 @@
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -744,7 +744,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -755,7 +755,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0.3923611111111111</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -777,7 +777,7 @@
         <v>0.39583333333333331</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -788,7 +788,7 @@
         <v>0.42708333333333331</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -799,7 +799,7 @@
         <v>0.43402777777777779</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -810,7 +810,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -821,7 +821,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -843,7 +843,7 @@
         <v>0.47222222222222221</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -854,7 +854,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -865,7 +865,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -876,7 +876,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -887,7 +887,7 @@
         <v>0.68055555555555558</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -898,7 +898,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -920,7 +920,7 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>

</xml_diff>